<commit_message>
realizando mejoras visuales a los archivos excel y pdf
</commit_message>
<xml_diff>
--- a/coeSap.xlsx
+++ b/coeSap.xlsx
@@ -22,10 +22,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t xml:space="preserve">
-CORTES DE VENTAS DE COEDICIONES
-SIGLO DEL HOMBRE EDITORES S.A
-NIT. 800.154.368-8</t>
+    <t xml:space="preserve">SIGLO DEL HOMBRE EDITORES S.A
+NIT. 800.154.368-8
+CORTES DE VENTAS DE COEDICIONES</t>
   </si>
   <si>
     <t xml:space="preserve">Periodo: Junio 1 de 2023 a Junio 30 de 2023 - VENTAS NACIONALES    </t>
@@ -70,10 +69,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="165" formatCode="[$$-240A]#,##0.00;[RED]\([$$-240A]#,##0.00\)"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -95,6 +94,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -222,7 +227,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -243,11 +248,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -279,7 +284,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -367,9 +372,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1402200</xdr:colOff>
+      <xdr:colOff>1401480</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>110880</xdr:rowOff>
+      <xdr:rowOff>110160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -383,7 +388,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="651240" y="533520"/>
-          <a:ext cx="750960" cy="747000"/>
+          <a:ext cx="750240" cy="746280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -406,7 +411,11 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="54" zoomScaleNormal="54" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <pane xSplit="5" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -416,10 +425,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="32.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="11.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="20.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="21.44"/>
   </cols>
   <sheetData>
@@ -488,16 +497,16 @@
       <c r="F4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="10" t="s">
         <v>11</v>
       </c>
       <c r="K4" s="11" t="s">

</xml_diff>